<commit_message>
Fixed corupt workbook input file for pandas
</commit_message>
<xml_diff>
--- a/StationCode_Torque Media.xlsx
+++ b/StationCode_Torque Media.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\python\excel-xml-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44B364E-F9A5-406F-8BDC-2FE555CA73C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2A625F-D7F3-44ED-A83C-B43CD362F867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="331">
   <si>
     <t>ALX</t>
   </si>
@@ -286,9 +286,6 @@
     <t>KOV</t>
   </si>
   <si>
-    <t>1584</t>
-  </si>
-  <si>
     <t>ENER</t>
   </si>
   <si>
@@ -950,9 +947,6 @@
   </si>
   <si>
     <t>SOW</t>
-  </si>
-  <si>
-    <t>R78</t>
   </si>
   <si>
     <t>ESTW</t>
@@ -1025,9 +1019,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0;[Red]&quot;R&quot;\ \-#,##0"/>
-  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1519,7 +1510,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1530,7 +1521,6 @@
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1544,9 +1534,6 @@
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1928,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C259"/>
+  <dimension ref="A1:C257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:XFD133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,10 +1930,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1960,19 +1947,19 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>104</v>
+        <v>173</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -1990,52 +1977,52 @@
         <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>312</v>
+      <c r="A10" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>312</v>
+      <c r="A11" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -2050,7 +2037,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>85</v>
@@ -2059,16 +2046,16 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
@@ -2077,27 +2064,27 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>320</v>
+      <c r="A18" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>318</v>
       </c>
       <c r="C18" s="3"/>
     </row>
@@ -2106,7 +2093,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="3"/>
     </row>
@@ -2121,145 +2108,145 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>323</v>
+      <c r="A23" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>321</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>303</v>
+      <c r="A25" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>302</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>302</v>
+      <c r="A27" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>301</v>
       </c>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>289</v>
+      <c r="A29" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>288</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>318</v>
+      <c r="A31" s="5" t="s">
+        <v>316</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>105</v>
+        <v>174</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>322</v>
+      <c r="A34" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>106</v>
+        <v>175</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C36" s="3"/>
     </row>
@@ -2268,43 +2255,43 @@
         <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>107</v>
+        <v>176</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>212</v>
+      <c r="A39" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>301</v>
+      <c r="A40" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>300</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C41" s="3"/>
     </row>
@@ -2318,29 +2305,29 @@
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>109</v>
+        <v>178</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C45" s="3"/>
     </row>
@@ -2348,44 +2335,44 @@
       <c r="A46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>319</v>
+      <c r="A47" s="5" t="s">
+        <v>317</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C47" s="12"/>
+        <v>317</v>
+      </c>
+      <c r="C47" s="10"/>
     </row>
     <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C50" s="3"/>
     </row>
@@ -2400,7 +2387,7 @@
     </row>
     <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>68</v>
@@ -2409,52 +2396,52 @@
     </row>
     <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>316</v>
+        <v>179</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>314</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>110</v>
+        <v>180</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>9</v>
@@ -2462,10 +2449,10 @@
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="3"/>
@@ -2475,7 +2462,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C60" s="3"/>
     </row>
@@ -2490,10 +2477,10 @@
     </row>
     <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C62" s="3"/>
     </row>
@@ -2502,16 +2489,16 @@
         <v>13</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>112</v>
+        <v>182</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C64" s="3"/>
     </row>
@@ -2526,55 +2513,55 @@
     </row>
     <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>113</v>
+        <v>183</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>114</v>
+        <v>184</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C71" s="3"/>
     </row>
@@ -2582,62 +2569,62 @@
       <c r="A72" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C72" s="3"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C74" s="3"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>115</v>
+        <v>185</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="C75" s="3"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C78" s="3"/>
     </row>
@@ -2651,20 +2638,20 @@
       <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="6" t="s">
+      <c r="B80" s="5" t="s">
         <v>70</v>
       </c>
       <c r="C80" s="3"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>141</v>
+      <c r="A81" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="C81" s="3"/>
     </row>
@@ -2679,10 +2666,10 @@
     </row>
     <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="C83" s="3"/>
     </row>
@@ -2697,79 +2684,79 @@
     </row>
     <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>117</v>
+        <v>186</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>118</v>
+        <v>187</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>119</v>
+        <v>189</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C91" s="3"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B92" s="6" t="s">
-        <v>142</v>
+        <v>203</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>18</v>
@@ -2777,56 +2764,56 @@
       <c r="C93" s="3"/>
     </row>
     <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="B94" s="6" t="s">
-        <v>329</v>
+      <c r="A94" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>327</v>
       </c>
       <c r="C94" s="3"/>
     </row>
     <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="B95" s="6" t="s">
+      <c r="A95" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C95" s="3"/>
     </row>
     <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B96" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C96" s="3"/>
     </row>
     <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C97" s="3"/>
     </row>
     <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>120</v>
+        <v>191</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="C98" s="3"/>
     </row>
     <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B99" s="6" t="s">
-        <v>299</v>
+      <c r="A99" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>298</v>
       </c>
       <c r="C99" s="3"/>
     </row>
@@ -2840,47 +2827,47 @@
       <c r="C100" s="3"/>
     </row>
     <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B101" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C102" s="3"/>
     </row>
     <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C103" s="3"/>
     </row>
     <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>121</v>
+        <v>192</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="C104" s="3"/>
     </row>
     <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C105" s="3"/>
     </row>
@@ -2895,7 +2882,7 @@
     </row>
     <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>72</v>
@@ -2913,19 +2900,19 @@
     </row>
     <row r="109" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B109" s="6" t="s">
-        <v>122</v>
+        <v>193</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B110" s="6" t="s">
-        <v>123</v>
+        <v>194</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="C110" s="3"/>
     </row>
@@ -2940,16 +2927,16 @@
     </row>
     <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C112" s="3"/>
     </row>
     <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>50</v>
@@ -2957,35 +2944,35 @@
       <c r="C113" s="3"/>
     </row>
     <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>298</v>
+      <c r="A114" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>297</v>
       </c>
       <c r="C114" s="3"/>
     </row>
     <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C115" s="3"/>
     </row>
     <row r="116" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C116" s="3"/>
     </row>
     <row r="117" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>44</v>
@@ -2994,28 +2981,28 @@
     </row>
     <row r="118" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C118" s="3"/>
     </row>
     <row r="119" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C119" s="3"/>
     </row>
     <row r="120" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A120" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>313</v>
+      <c r="A120" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>311</v>
       </c>
       <c r="C120" s="2"/>
     </row>
@@ -3030,25 +3017,25 @@
     </row>
     <row r="122" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C122" s="3"/>
     </row>
     <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C123" s="3"/>
     </row>
     <row r="124" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>25</v>
@@ -3057,55 +3044,55 @@
     </row>
     <row r="125" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C125" s="3"/>
     </row>
     <row r="126" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C126" s="3"/>
     </row>
     <row r="127" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="B127" s="8" t="s">
-        <v>214</v>
+      <c r="A127" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="C127" s="3"/>
     </row>
     <row r="128" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C128" s="3"/>
     </row>
     <row r="129" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>125</v>
+        <v>196</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C129" s="3"/>
     </row>
     <row r="130" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C130" s="3"/>
     </row>
@@ -3119,182 +3106,182 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="1">
-        <v>1584</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>88</v>
+      <c r="A132" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="C132" s="3"/>
     </row>
     <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
-        <v>786</v>
-      </c>
-      <c r="B133" s="11" t="s">
-        <v>310</v>
+      <c r="A133" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>273</v>
       </c>
       <c r="C133" s="3"/>
     </row>
     <row r="134" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>145</v>
+        <v>218</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>273</v>
+        <v>218</v>
       </c>
       <c r="C134" s="3"/>
     </row>
     <row r="135" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C135" s="3"/>
     </row>
     <row r="136" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>219</v>
+      <c r="A136" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="C136" s="3"/>
     </row>
     <row r="137" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>277</v>
+        <v>88</v>
       </c>
       <c r="C137" s="3"/>
     </row>
     <row r="138" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A138" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B138" s="8" t="s">
-        <v>89</v>
+      <c r="A138" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="C138" s="3"/>
     </row>
     <row r="139" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>89</v>
+        <v>216</v>
       </c>
       <c r="C139" s="3"/>
     </row>
     <row r="140" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B140" s="6" t="s">
-        <v>108</v>
+        <v>150</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>278</v>
       </c>
       <c r="C140" s="3"/>
     </row>
     <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="C141" s="3"/>
     </row>
     <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>279</v>
+        <v>63</v>
       </c>
       <c r="C142" s="3"/>
     </row>
     <row r="143" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>152</v>
+        <v>8</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>280</v>
+        <v>8</v>
       </c>
       <c r="C143" s="3"/>
     </row>
     <row r="144" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>63</v>
+        <v>328</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C144" s="3"/>
     </row>
     <row r="145" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>8</v>
+        <v>305</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>8</v>
+        <v>181</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="C146" s="3"/>
     </row>
     <row r="147" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>306</v>
+        <v>89</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="C147" s="3"/>
     </row>
     <row r="148" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>111</v>
+        <v>217</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="C148" s="3"/>
     </row>
     <row r="149" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>281</v>
+        <v>154</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>218</v>
+        <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>218</v>
+        <v>155</v>
       </c>
       <c r="C150" s="3"/>
     </row>
     <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>307</v>
+        <v>14</v>
       </c>
       <c r="C151" s="3"/>
     </row>
@@ -3303,178 +3290,178 @@
         <v>156</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="C152" s="3"/>
     </row>
     <row r="153" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>15</v>
+        <v>221</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="C154" s="3"/>
     </row>
     <row r="155" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>64</v>
+        <v>281</v>
       </c>
       <c r="C155" s="3"/>
     </row>
     <row r="156" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>91</v>
+        <v>210</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>271</v>
       </c>
       <c r="C156" s="3"/>
     </row>
     <row r="157" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>17</v>
+        <v>159</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>211</v>
+        <v>48</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>272</v>
+        <v>48</v>
       </c>
       <c r="C158" s="3"/>
     </row>
     <row r="159" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>284</v>
+        <v>22</v>
       </c>
       <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C160" s="3"/>
     </row>
     <row r="161" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>22</v>
+        <v>219</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>22</v>
+        <v>219</v>
       </c>
       <c r="C161" s="3"/>
     </row>
     <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>23</v>
+        <v>284</v>
       </c>
       <c r="C162" s="3"/>
     </row>
     <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>220</v>
+      <c r="A163" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>162</v>
+        <v>220</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>285</v>
+        <v>220</v>
       </c>
       <c r="C164" s="3"/>
     </row>
     <row r="165" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B165" s="6" t="s">
-        <v>73</v>
+      <c r="A165" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>221</v>
+        <v>195</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C166" s="3"/>
     </row>
     <row r="167" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="B167" s="9" t="s">
-        <v>213</v>
+      <c r="A167" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B168" s="6" t="s">
-        <v>124</v>
+        <v>27</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>285</v>
       </c>
       <c r="C168" s="3"/>
     </row>
     <row r="169" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>286</v>
+        <v>307</v>
       </c>
       <c r="C170" s="3"/>
     </row>
     <row r="171" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>51</v>
+        <v>91</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="C171" s="3"/>
     </row>
@@ -3483,792 +3470,774 @@
         <v>166</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>308</v>
+        <v>53</v>
       </c>
       <c r="C172" s="3"/>
     </row>
     <row r="173" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>92</v>
+        <v>167</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C173" s="3"/>
     </row>
     <row r="174" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>53</v>
+        <v>214</v>
       </c>
       <c r="C174" s="3"/>
     </row>
     <row r="175" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>29</v>
+        <v>308</v>
       </c>
       <c r="C175" s="3"/>
     </row>
     <row r="176" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="C176" s="3"/>
     </row>
     <row r="177" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>309</v>
+        <v>168</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="C177" s="3"/>
     </row>
     <row r="178" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>236</v>
+        <v>30</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
       <c r="C178" s="3"/>
     </row>
     <row r="179" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>287</v>
+        <v>78</v>
       </c>
       <c r="C180" s="3"/>
     </row>
     <row r="181" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C182" s="3"/>
     </row>
     <row r="183" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>58</v>
+        <v>282</v>
       </c>
       <c r="C184" s="3"/>
     </row>
     <row r="185" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="C185" s="3"/>
     </row>
     <row r="186" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>283</v>
+        <v>40</v>
       </c>
       <c r="C186" s="3"/>
     </row>
     <row r="187" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>324</v>
+        <v>215</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>324</v>
+        <v>215</v>
       </c>
       <c r="C187" s="3"/>
     </row>
     <row r="188" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>205</v>
+        <v>41</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C188" s="3"/>
     </row>
     <row r="189" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>216</v>
+        <v>52</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C189" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="C189" s="9"/>
     </row>
     <row r="190" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>41</v>
+        <v>315</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C190" s="3"/>
+        <v>315</v>
+      </c>
+      <c r="C190" s="9"/>
     </row>
     <row r="191" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C191" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C191" s="3"/>
     </row>
     <row r="192" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>317</v>
+        <v>74</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C192" s="10"/>
+        <v>74</v>
+      </c>
+      <c r="C192" s="3"/>
     </row>
     <row r="193" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>94</v>
+        <v>266</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="C193" s="3"/>
     </row>
     <row r="194" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>74</v>
+        <v>265</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>74</v>
+        <v>265</v>
       </c>
       <c r="C194" s="3"/>
     </row>
     <row r="195" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>267</v>
+      <c r="A195" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>325</v>
       </c>
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>266</v>
+      <c r="A196" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>312</v>
       </c>
       <c r="C196" s="3"/>
     </row>
     <row r="197" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="B197" s="6" t="s">
-        <v>327</v>
+      <c r="A197" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C197" s="3"/>
     </row>
     <row r="198" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A198" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>314</v>
+      <c r="A198" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C198" s="3"/>
     </row>
     <row r="199" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
       <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>55</v>
+        <v>87</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="C200" s="3"/>
     </row>
     <row r="201" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="C201" s="3"/>
     </row>
     <row r="202" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B202" s="6" t="s">
-        <v>126</v>
+      <c r="A202" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B202" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="C202" s="3"/>
     </row>
     <row r="203" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>137</v>
+      <c r="A203" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>292</v>
       </c>
       <c r="C203" s="3"/>
     </row>
     <row r="204" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="B204" s="8" t="s">
-        <v>208</v>
+      <c r="A204" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C204" s="3"/>
     </row>
     <row r="205" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A205" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="B205" s="8" t="s">
-        <v>293</v>
+      <c r="A205" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="C205" s="3"/>
     </row>
     <row r="206" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A206" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B206" s="6" t="s">
-        <v>76</v>
+      <c r="A206" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="C206" s="3"/>
     </row>
     <row r="207" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>93</v>
+        <v>267</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>77</v>
+        <v>267</v>
       </c>
       <c r="C207" s="3"/>
     </row>
     <row r="208" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>297</v>
+        <v>132</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>297</v>
+        <v>236</v>
       </c>
       <c r="C208" s="3"/>
     </row>
     <row r="209" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>268</v>
+      <c r="A209" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="C209" s="3"/>
     </row>
     <row r="210" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A210" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>237</v>
+      <c r="A210" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="C210" s="3"/>
     </row>
     <row r="211" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A211" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B211" s="6" t="s">
-        <v>237</v>
+      <c r="A211" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C211" s="3"/>
     </row>
     <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A212" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>237</v>
+      <c r="A212" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="C212" s="3"/>
     </row>
     <row r="213" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>31</v>
+        <v>198</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C213" s="3"/>
     </row>
     <row r="214" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>95</v>
+        <v>199</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C214" s="3"/>
     </row>
     <row r="215" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B215" s="6" t="s">
-        <v>127</v>
+        <v>171</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C215" s="3"/>
     </row>
     <row r="216" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A216" s="1" t="s">
+      <c r="A216" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C216" s="3"/>
+    </row>
+    <row r="217" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C217" s="3"/>
+    </row>
+    <row r="218" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C218" s="3"/>
+    </row>
+    <row r="219" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B216" s="6" t="s">
+      <c r="B219" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C216" s="3"/>
-    </row>
-    <row r="217" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A217" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C217" s="3"/>
-    </row>
-    <row r="218" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A218" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B218" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C218" s="3"/>
-    </row>
-    <row r="219" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A219" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B219" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="C219" s="3"/>
     </row>
     <row r="220" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A220" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>60</v>
+      <c r="A220" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="C220" s="3"/>
     </row>
     <row r="221" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B221" s="6" t="s">
-        <v>129</v>
+      <c r="A221" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="C221" s="3"/>
     </row>
     <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>130</v>
+        <v>33</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C222" s="3"/>
     </row>
     <row r="223" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A223" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B223" s="6" t="s">
-        <v>79</v>
+      <c r="A223" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C223" s="3"/>
     </row>
     <row r="224" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>288</v>
+        <v>35</v>
       </c>
       <c r="C224" s="3"/>
     </row>
     <row r="225" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>36</v>
+      <c r="A225" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C225" s="3"/>
     </row>
     <row r="226" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>35</v>
+        <v>230</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>35</v>
+        <v>230</v>
       </c>
       <c r="C226" s="3"/>
     </row>
     <row r="227" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B227" s="6" t="s">
-        <v>61</v>
+      <c r="A227" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="C227" s="3"/>
     </row>
     <row r="228" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>231</v>
+        <v>37</v>
       </c>
       <c r="C228" s="3"/>
     </row>
     <row r="229" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B229" s="5" t="s">
-        <v>96</v>
+        <v>260</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="C229" s="3"/>
     </row>
     <row r="230" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C230" s="3"/>
     </row>
     <row r="231" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>261</v>
+        <v>38</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>261</v>
+        <v>38</v>
       </c>
       <c r="C231" s="3"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C232" s="3"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="C233" s="3"/>
     </row>
-    <row r="234" spans="1:3" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="C234" s="3"/>
     </row>
-    <row r="235" spans="1:3" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>269</v>
+    <row r="235" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A235" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C235" s="3"/>
     </row>
     <row r="236" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>209</v>
+      <c r="A236" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="C236" s="3"/>
     </row>
     <row r="237" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A237" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B237" s="6" t="s">
-        <v>131</v>
+      <c r="A237" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="C237" s="3"/>
     </row>
     <row r="238" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A238" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>80</v>
+      <c r="A238" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>299</v>
       </c>
       <c r="C238" s="3"/>
     </row>
     <row r="239" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>232</v>
+      <c r="A239" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C239" s="3"/>
     </row>
     <row r="240" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A240" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B240" s="6" t="s">
-        <v>300</v>
+      <c r="A240" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C240" s="3"/>
     </row>
     <row r="241" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A241" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B241" s="6" t="s">
-        <v>42</v>
+      <c r="A241" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C241" s="3"/>
     </row>
     <row r="242" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A242" s="6" t="s">
-        <v>315</v>
+      <c r="A242" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="B242" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C242" s="3"/>
+    </row>
+    <row r="243" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A243" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C243" s="3"/>
+    </row>
+    <row r="244" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C244" s="3"/>
+    </row>
+    <row r="245" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A245" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C245" s="3"/>
+    </row>
+    <row r="246" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C246" s="3"/>
+    </row>
+    <row r="247" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C247" s="3"/>
+    </row>
+    <row r="248" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A248" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C248" s="3"/>
+    </row>
+    <row r="249" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A249" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C249" s="3"/>
+    </row>
+    <row r="250" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A250" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C250" s="3"/>
+    </row>
+    <row r="251" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A251" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C251" s="3"/>
+    </row>
+    <row r="252" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A252" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C252" s="3"/>
+    </row>
+    <row r="253" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A253" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C253" s="3"/>
+    </row>
+    <row r="254" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A254" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C254" s="3"/>
+    </row>
+    <row r="255" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A255" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C255" s="3"/>
+    </row>
+    <row r="256" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A256" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C242" s="3"/>
-    </row>
-    <row r="243" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A243" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C243" s="3"/>
-    </row>
-    <row r="244" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A244" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B244" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C244" s="3"/>
-    </row>
-    <row r="245" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A245" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B245" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C245" s="3"/>
-    </row>
-    <row r="246" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A246" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C246" s="3"/>
-    </row>
-    <row r="247" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A247" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C247" s="3"/>
-    </row>
-    <row r="248" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A248" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C248" s="3"/>
-    </row>
-    <row r="249" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C249" s="3"/>
-    </row>
-    <row r="250" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A250" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C250" s="3"/>
-    </row>
-    <row r="251" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A251" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C251" s="3"/>
-    </row>
-    <row r="252" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A252" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C252" s="3"/>
-    </row>
-    <row r="253" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A253" s="6" t="s">
+      <c r="B256" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C256" s="3"/>
+    </row>
+    <row r="257" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A257" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C253" s="3"/>
-    </row>
-    <row r="254" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A254" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C254" s="3"/>
-    </row>
-    <row r="255" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A255" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C255" s="3"/>
-    </row>
-    <row r="256" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A256" s="6" t="s">
+      <c r="B257" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B256" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C256" s="3"/>
-    </row>
-    <row r="257" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A257" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C257" s="3"/>
-    </row>
-    <row r="258" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A258" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C258" s="3"/>
-    </row>
-    <row r="259" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A259" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C259" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>